<commit_message>
added DEM column for easy use
</commit_message>
<xml_diff>
--- a/Low head Dam Info - Copy for python.xlsx
+++ b/Low head Dam Info - Copy for python.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\DHS_LowHeadDam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C3F00-F272-4B32-95E3-76E368EBAF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93B188B-7971-47E8-B9DB-405E2B9D515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="192" windowWidth="13092" windowHeight="9408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slopes" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4580" uniqueCount="1766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4581" uniqueCount="1767">
   <si>
     <t>ID</t>
   </si>
@@ -5632,6 +5632,9 @@
   </si>
   <si>
     <t>gpkg</t>
+  </si>
+  <si>
+    <t>DEM</t>
   </si>
 </sst>
 </file>
@@ -6194,17 +6197,18 @@
   <dimension ref="A1:AG919"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.44140625" customWidth="1"/>
@@ -6279,7 +6283,9 @@
       <c r="Y1" s="3" t="s">
         <v>1765</v>
       </c>
-      <c r="Z1" s="3"/>
+      <c r="Z1" s="3" t="s">
+        <v>1766</v>
+      </c>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
@@ -68629,6 +68635,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AE0E7A75C7BE64682F04F88A6283C3D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a35657f5e79cca0b21d99089b5ab184">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04098f7e-c17d-4d50-9dd7-02de032a1f4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9891b2a79765bcd974795441df6ae999" ns2:_="">
     <xsd:import namespace="04098f7e-c17d-4d50-9dd7-02de032a1f4d"/>
@@ -68772,22 +68793,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D86D56-EE4C-49E2-AC68-E8BE0529A6FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68803,21 +68826,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
took out DEM column since had errors
</commit_message>
<xml_diff>
--- a/Low head Dam Info - Copy for python.xlsx
+++ b/Low head Dam Info - Copy for python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\DHS_LowHeadDam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93B188B-7971-47E8-B9DB-405E2B9D515C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B93A6A-7017-4C9F-B886-52149AF1C60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="192" windowWidth="13092" windowHeight="9408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4581" uniqueCount="1767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4580" uniqueCount="1766">
   <si>
     <t>ID</t>
   </si>
@@ -5632,9 +5632,6 @@
   </si>
   <si>
     <t>gpkg</t>
-  </si>
-  <si>
-    <t>DEM</t>
   </si>
 </sst>
 </file>
@@ -6197,7 +6194,7 @@
   <dimension ref="A1:AG919"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Z6" sqref="Z6"/>
@@ -6283,9 +6280,7 @@
       <c r="Y1" s="3" t="s">
         <v>1765</v>
       </c>
-      <c r="Z1" s="3" t="s">
-        <v>1766</v>
-      </c>
+      <c r="Z1" s="3"/>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>

</xml_diff>

<commit_message>
added DEM column back in
</commit_message>
<xml_diff>
--- a/Low head Dam Info - Copy for python.xlsx
+++ b/Low head Dam Info - Copy for python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\DHS_LowHeadDam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B93A6A-7017-4C9F-B886-52149AF1C60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E105B9-A209-406C-8796-218B210F67FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="192" windowWidth="13092" windowHeight="9408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4580" uniqueCount="1766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4581" uniqueCount="1767">
   <si>
     <t>ID</t>
   </si>
@@ -5632,6 +5632,9 @@
   </si>
   <si>
     <t>gpkg</t>
+  </si>
+  <si>
+    <t>DEM</t>
   </si>
 </sst>
 </file>
@@ -6280,7 +6283,9 @@
       <c r="Y1" s="3" t="s">
         <v>1765</v>
       </c>
-      <c r="Z1" s="3"/>
+      <c r="Z1" s="3" t="s">
+        <v>1766</v>
+      </c>
       <c r="AA1" s="3"/>
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
@@ -68630,21 +68635,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AE0E7A75C7BE64682F04F88A6283C3D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a35657f5e79cca0b21d99089b5ab184">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04098f7e-c17d-4d50-9dd7-02de032a1f4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9891b2a79765bcd974795441df6ae999" ns2:_="">
     <xsd:import namespace="04098f7e-c17d-4d50-9dd7-02de032a1f4d"/>
@@ -68788,24 +68778,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D86D56-EE4C-49E2-AC68-E8BE0529A6FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68821,4 +68809,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
expanded the left-side columns (nothing major changed)
</commit_message>
<xml_diff>
--- a/Low head Dam Info - Copy for python.xlsx
+++ b/Low head Dam Info - Copy for python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\DHS_LowHeadDam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E105B9-A209-406C-8796-218B210F67FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6392C0-9BFF-4DC5-9C03-2370743AA432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="192" windowWidth="13092" windowHeight="9408" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Slopes" sheetId="1" r:id="rId1"/>
@@ -6197,7 +6197,7 @@
   <dimension ref="A1:AG919"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Z6" sqref="Z6"/>
@@ -6206,9 +6206,9 @@
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="62.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.44140625" customWidth="1"/>
@@ -68635,6 +68635,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005AE0E7A75C7BE64682F04F88A6283C3D" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a35657f5e79cca0b21d99089b5ab184">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="04098f7e-c17d-4d50-9dd7-02de032a1f4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9891b2a79765bcd974795441df6ae999" ns2:_="">
     <xsd:import namespace="04098f7e-c17d-4d50-9dd7-02de032a1f4d"/>
@@ -68778,22 +68793,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45D86D56-EE4C-49E2-AC68-E8BE0529A6FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -68809,21 +68826,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE075FDA-3081-4C63-B5D0-FD605F0909E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7192B276-84C5-4A31-8E4E-D0B5251E50AA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>